<commit_message>
BB-22361: Impossible to add product to Quick Order Form when multiple sellers have the same product SKU (#35178)
</commit_message>
<xml_diff>
--- a/src/Oro/Bundle/ProductBundle/Tests/Functional/Model/Builder/data/quick-order.xlsx
+++ b/src/Oro/Bundle/ProductBundle/Tests/Functional/Model/Builder/data/quick-order.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,13 +31,13 @@
     <t xml:space="preserve">Unit</t>
   </si>
   <si>
-    <t xml:space="preserve">1ABSC</t>
+    <t xml:space="preserve">product-1</t>
   </si>
   <si>
     <t xml:space="preserve">item</t>
   </si>
   <si>
-    <t xml:space="preserve">2ABSC</t>
+    <t xml:space="preserve">product-2</t>
   </si>
 </sst>
 </file>
@@ -128,32 +128,31 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Z3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="26" min="7" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -260,8 +259,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>